<commit_message>
rajout de synthese à la base reporting
</commit_message>
<xml_diff>
--- a/1.indata/base_garanties.xlsx
+++ b/1.indata/base_garanties.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\20250607 Indexation - neosoft\1.Original data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\20250607 Indexation - mutuelle vebcn\1.indata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22515472-F792-4CBD-BF29-890B8B6358AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9062188A-3155-48D8-BA9B-F109DC8DC818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{6F3450D7-4873-4DB7-9634-E24643DF0CFE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6F3450D7-4873-4DB7-9634-E24643DF0CFE}"/>
   </bookViews>
   <sheets>
     <sheet name="Garanties" sheetId="2" r:id="rId1"/>
@@ -1001,7 +1001,7 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1810,7 +1810,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Milliers" xfId="2" builtinId="3"/>
@@ -2235,7 +2235,9 @@
   </sheetPr>
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -4544,7 +4546,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AF7487-B74F-48A2-9647-5FC74E92FBEA}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>

</xml_diff>